<commit_message>
Update file -- adding conent
</commit_message>
<xml_diff>
--- a/HRMS_Microservice-Architecture.xlsx
+++ b/HRMS_Microservice-Architecture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zProfessional_Projects\ms-architecture-and-components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469234A3-6E21-4498-B517-BEC85DA79365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECDC1A4-B117-4DAC-9BE5-9A71EF291B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macro Level" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="ELK Arch" sheetId="5" r:id="rId4"/>
     <sheet name="Web MS Arch" sheetId="6" r:id="rId5"/>
     <sheet name="MS Txn Pattern" sheetId="8" r:id="rId6"/>
-    <sheet name="Docker Study" sheetId="7" r:id="rId7"/>
-    <sheet name="Log Tools Study Links" sheetId="3" r:id="rId8"/>
+    <sheet name="Common QA" sheetId="9" r:id="rId7"/>
+    <sheet name="Docker Study" sheetId="7" r:id="rId8"/>
+    <sheet name="Log Tools Study Links" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="148">
   <si>
     <t>Modules</t>
   </si>
@@ -79,9 +80,6 @@
     <t>iRecruitment Service</t>
   </si>
   <si>
-    <t>Reports</t>
-  </si>
-  <si>
     <t>Config Server</t>
   </si>
   <si>
@@ -101,9 +99,6 @@
   </si>
   <si>
     <t>Current Ternds</t>
-  </si>
-  <si>
-    <t>Spring Cloud Gateway</t>
   </si>
   <si>
     <t>Resilence 4j</t>
@@ -215,9 +210,6 @@
     <t>Spring Cloud Config</t>
   </si>
   <si>
-    <t>Elasticsearch is no SQL database</t>
-  </si>
-  <si>
     <t>https://www.javainuse.com/spring/springboot-microservice-elk</t>
   </si>
   <si>
@@ -284,9 +276,6 @@
     <t>https://dzone.com/articles/practical-transaction-handling-in-microservice-arc</t>
   </si>
   <si>
-    <t>Circuit beaker</t>
-  </si>
-  <si>
     <t>Not default</t>
   </si>
   <si>
@@ -299,27 +288,207 @@
     <t>Netflix Hystrix</t>
   </si>
   <si>
-    <t>On-Tour, Short Leave, Leave, Off Day Bill Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Master Config --&gt; Calender and Shift </t>
-  </si>
-  <si>
-    <t>Circuit 
-Breaker</t>
-  </si>
-  <si>
     <t>Transaction Management in Microservice Architecture</t>
   </si>
   <si>
     <t>Design Pattern</t>
+  </si>
+  <si>
+    <t>How to Handle fault talerance in micro service???</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Earlir</t>
+  </si>
+  <si>
+    <t>Hystrix</t>
+  </si>
+  <si>
+    <t>How to do distributed tracking in microservices???</t>
+  </si>
+  <si>
+    <t>Why we use Zull Gateway in Microservices??</t>
+  </si>
+  <si>
+    <t>Authentication and Security</t>
+  </si>
+  <si>
+    <t>insigght and monitoring</t>
+  </si>
+  <si>
+    <t>dynamic routing</t>
+  </si>
+  <si>
+    <t>Load balancing</t>
+  </si>
+  <si>
+    <t>What is the entry point of microservices???</t>
+  </si>
+  <si>
+    <t>what Design patter used in mircoservice ??</t>
+  </si>
+  <si>
+    <t>Domian driven?? Event Driven ?? Saga ?? CQRS</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sZCprZNqNTw</t>
+  </si>
+  <si>
+    <t>Event Sourcing ???</t>
+  </si>
+  <si>
+    <t>How to handle microservice scalling???</t>
+  </si>
+  <si>
+    <t>Deaploy customer microservice in multiple instance??</t>
+  </si>
+  <si>
+    <t>suppor custmer microservice has more load</t>
+  </si>
+  <si>
+    <t>What is the default message size Kafka accept???</t>
+  </si>
+  <si>
+    <t>Kafka configuration limits the size of messages that it's allowed to send. By default, this limit is 1MB</t>
+  </si>
+  <si>
+    <t>Replication factor in Kafka??</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=G0waumbpK48&amp;t=233s</t>
+  </si>
+  <si>
+    <t>Best Prictise in Microservices??</t>
+  </si>
+  <si>
+    <t>1. Individual DB</t>
+  </si>
+  <si>
+    <t>2. Indepdendent deployment</t>
+  </si>
+  <si>
+    <t>3. Indepentdent Build</t>
+  </si>
+  <si>
+    <t>4. Docerization</t>
+  </si>
+  <si>
+    <t>Experience in Micro-services (event driven microservices and spring boot)</t>
+  </si>
+  <si>
+    <t>What I learned from using Event Driven Architecture and DDD</t>
+  </si>
+  <si>
+    <t>what is the difference between event driven and domain driven design Microservices?</t>
+  </si>
+  <si>
+    <t>Event sourcing and domain events can of course be used both at the same time, but should not influence each other. The two concepts are used for different purposes and should therefore not be mixed.</t>
+  </si>
+  <si>
+    <t>In general, DDD is a methodology for creating complex software from a technical perspective. DDD gives us a bunch of building blocks for correct implementation of domain business logic. It handles the project also from a business perspective (strategic domain driven design). This approach puts stress on connecting these two worlds through some particular rules:</t>
+  </si>
+  <si>
+    <t>https://medium.com/briisk/what-i-learned-from-using-event-driven-architecture-and-ddd-ab154eeba489</t>
+  </si>
+  <si>
+    <t>Domain-Driven Design and Event-Driven Architecture</t>
+  </si>
+  <si>
+    <t>Fallbak Controller / Fault Talerance</t>
+  </si>
+  <si>
+    <t>https://javatechonline.com/how-to-implement-fault-tolerance-in-microservices-using-resilience4j/</t>
+  </si>
+  <si>
+    <t>https://medium.com/swlh/hystrix-fault-tolerance-and-circuit-breaker-for-spring-boot-38c744647acb</t>
+  </si>
+  <si>
+    <t>https://www.springboottutorial.com/fault-tolerance-in-microservices</t>
+  </si>
+  <si>
+    <t>https://www.classcentral.com/course/youtube-spring-boot-microservices-level-2-fault-tolerance-and-resilience-45738/classroom</t>
+  </si>
+  <si>
+    <t>Reports Service</t>
+  </si>
+  <si>
+    <t>Tracing</t>
+  </si>
+  <si>
+    <t>Fault Tolerance</t>
+  </si>
+  <si>
+    <t>Cental Log Management</t>
+  </si>
+  <si>
+    <t>H( Human ) R(Resouce) I(Information) S(System)</t>
+  </si>
+  <si>
+    <t>Device to collect punsh/finger print and Manage</t>
+  </si>
+  <si>
+    <t>Salary Processing</t>
+  </si>
+  <si>
+    <t>All kind of reports</t>
+  </si>
+  <si>
+    <t>On-Tour, Short Leave, Leave, Off Day Bill Processing, Transport Requisiotion, Gymnasium Requisition, Food Requistion</t>
+  </si>
+  <si>
+    <t>Master Config --&gt; Calender and Shift (A, B, C)</t>
+  </si>
+  <si>
+    <t>A=8 Hours (9:00 AM to 5:00PM)</t>
+  </si>
+  <si>
+    <t>B=8 Hours (5:00 PM to 1:00AM)</t>
+  </si>
+  <si>
+    <t>C=8 Hours (1:00 AM to 9:00AM)</t>
+  </si>
+  <si>
+    <t>Total 24 Hours</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>Eureka Server (For Service Discovery)</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>Sleuth and Zipkin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#5
+</t>
+  </si>
+  <si>
+    <t>Circuit Breaker</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>Elasticsearch is a no SQL database</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,8 +535,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,6 +554,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -541,12 +736,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -563,6 +752,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -574,6 +770,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1175,7 +1380,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>307655</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>708561</xdr:rowOff>
+      <xdr:rowOff>704751</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1217,7 +1422,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>250508</xdr:colOff>
+      <xdr:colOff>246698</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>1809</xdr:rowOff>
     </xdr:to>
@@ -1261,9 +1466,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>250502</xdr:colOff>
+      <xdr:colOff>246692</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>20829</xdr:rowOff>
+      <xdr:rowOff>17019</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1305,9 +1510,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>324801</xdr:colOff>
+      <xdr:colOff>320991</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>975233</xdr:rowOff>
+      <xdr:rowOff>971423</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1349,9 +1554,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>288608</xdr:colOff>
+      <xdr:colOff>284798</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>784764</xdr:rowOff>
+      <xdr:rowOff>780954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1395,7 +1600,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>305753</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>13236</xdr:rowOff>
+      <xdr:rowOff>17046</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1439,7 +1644,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>269559</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>22758</xdr:rowOff>
+      <xdr:rowOff>18948</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1481,9 +1686,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>168594</xdr:colOff>
+      <xdr:colOff>172404</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>55120</xdr:rowOff>
+      <xdr:rowOff>58930</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1616,16 +1821,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>43815</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>550545</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1905</xdr:rowOff>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>27587</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>520982</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>146255</xdr:rowOff>
+      <xdr:rowOff>150065</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1648,12 +1853,73 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1263015" y="733425"/>
-          <a:ext cx="7908572" cy="3436190"/>
+          <a:off x="550545" y="735330"/>
+          <a:ext cx="7897142" cy="3396185"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1905</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>55245</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74918C84-A555-E5A5-04CC-4165D5A293EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9124950" y="725805"/>
+          <a:ext cx="8648700" cy="5120640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1924,10 +2190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="X29" sqref="X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1937,19 +2203,19 @@
     <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="3"/>
@@ -1958,24 +2224,24 @@
       <c r="M3" s="3"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
       <c r="L4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
@@ -1984,14 +2250,14 @@
       <c r="M5" s="9"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
@@ -2004,9 +2270,9 @@
       <c r="L7" s="3"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
@@ -2019,7 +2285,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2031,7 +2297,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -2043,7 +2309,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11" s="12"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
@@ -2057,11 +2323,16 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="7"/>
-      <c r="P11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P11" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="T11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
@@ -2073,11 +2344,13 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="7"/>
-      <c r="P12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P12" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
@@ -2091,11 +2364,16 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="7"/>
-      <c r="P13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P13" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="T13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14" s="13"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
@@ -2109,11 +2387,16 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="7"/>
-      <c r="P14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P14" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="T14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
@@ -2126,7 +2409,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
         <v>8</v>
@@ -2213,7 +2496,7 @@
       <c r="B22" s="14"/>
       <c r="D22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="6"/>
@@ -2230,7 +2513,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="11" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -2315,62 +2598,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80096996-98D7-4360-BE99-E9CC6F38B3B4}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="2" max="2" width="105.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>88</v>
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2382,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40637708-2B42-412F-8D81-C6544A71098C}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2398,172 +2712,194 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="3" spans="1:12" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="7" spans="1:12" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+    </row>
+    <row r="10" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29"/>
+      <c r="B10" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+    </row>
+    <row r="12" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="34"/>
+    </row>
+    <row r="14" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="34" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19" t="s">
+      <c r="D14" s="17"/>
+      <c r="E14" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="16" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="7" spans="1:12" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
-      <c r="B9" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-    </row>
-    <row r="10" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-    </row>
-    <row r="12" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-    </row>
-    <row r="14" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-    </row>
-    <row r="16" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15" t="s">
+      <c r="C16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>59</v>
-      </c>
+      <c r="D16" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="J9:L10"/>
     <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2575,15 +2911,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC37CA48-3374-4035-BB82-94CFDB588F2E}">
   <dimension ref="C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="31" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2594,31 +2930,35 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E407D17-DBAB-49B6-A5FE-38D3C42CE712}">
-  <dimension ref="C2"/>
+  <dimension ref="B2:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
-        <v>85</v>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F07B5F9-FD28-47BE-8C18-265BAF352A96}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2627,8 +2967,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="23" t="s">
-        <v>90</v>
+      <c r="B1" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2636,7 +2976,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2644,50 +2984,58 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2697,43 +3045,244 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26CB8EB3-BA53-404E-9B5F-1F3B2EA60455}">
+  <dimension ref="A1:J61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" s="23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F39" s="23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5847794-F934-4795-8D94-110DA2009783}">
   <dimension ref="B2:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2741,12 +3290,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0E7E4E-CB1F-434E-8EE0-88AE064057AB}">
   <dimension ref="B1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,79 +3307,79 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="C6" s="17" t="s">
-        <v>40</v>
+      <c r="C6" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C17" s="18" t="s">
-        <v>62</v>
+      <c r="C17" s="16" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C21" s="15" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="C21" s="17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>